<commit_message>
limpie el codigo y le agregue mas categorias a keepa
</commit_message>
<xml_diff>
--- a/titulos_enviados_06-02-2025.xlsx
+++ b/titulos_enviados_06-02-2025.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -510,6 +510,41 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>No se encontró el título.</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Sony WH-1000XM4 Audífonos inalámbricos con Noise Cancelling, Negro (Versión Nacional)</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Sony WH-1000XM4 Audífonos inalámbricos con Noise Cancelling, Negro (Versión Nacional)</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>La agonía del eros</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Sony WH-1000XM4 Audífonos inalámbricos con Noise Cancelling, Negro (Versión Nacional)</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>